<commit_message>
Updated excel file and screenshots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -34,12 +34,73 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Vince</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Vincent Martin</t>
+  </si>
+  <si>
+    <t>vince@nadin.one</t>
+  </si>
+  <si>
+    <t>Chris95</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>Christopher Perrins</t>
+  </si>
+  <si>
+    <t>christopher.perrins@qa.com</t>
+  </si>
+  <si>
+    <t>M4TT</t>
+  </si>
+  <si>
+    <t>chick3nWing</t>
+  </si>
+  <si>
+    <t>matthewhunt</t>
+  </si>
+  <si>
+    <t>matthew.hunt@qa.com</t>
+  </si>
+  <si>
+    <t>D�v</t>
+  </si>
+  <si>
+    <t>D@T@</t>
+  </si>
+  <si>
+    <t>Dev Gonsai</t>
+  </si>
+  <si>
+    <t>dev.gonsai@qa.com</t>
+  </si>
+  <si>
+    <t>Matttt</t>
+  </si>
+  <si>
+    <t>chris@qa.com</t>
+  </si>
+  <si>
+    <t>matt@qa.com</t>
+  </si>
+  <si>
+    <t>dev@qa.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="A2:E6"/>
@@ -359,10 +420,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -382,6 +443,91 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
delete scenario added, working but not deleting from .xlsx file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -420,10 +420,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
now deleting from .xlsx file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -412,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="A2:E6"/>
@@ -443,91 +443,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>